<commit_message>
separando permição no front e começando os relatórios
</commit_message>
<xml_diff>
--- a/projeto teste/docs/cronograma.xlsx
+++ b/projeto teste/docs/cronograma.xlsx
@@ -461,6 +461,31 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -476,34 +501,9 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
@@ -790,7 +790,7 @@
   <dimension ref="A1:AR35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AJ13" sqref="AJ13"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,270 +799,270 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="39" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="40"/>
-      <c r="AG1" s="40"/>
-      <c r="AH1" s="40"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
     </row>
     <row r="2" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
-      <c r="AC2" s="40"/>
-      <c r="AD2" s="40"/>
-      <c r="AE2" s="40"/>
-      <c r="AF2" s="40"/>
-      <c r="AG2" s="40"/>
-      <c r="AH2" s="40"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="51"/>
+      <c r="AB2" s="51"/>
+      <c r="AC2" s="51"/>
+      <c r="AD2" s="51"/>
+      <c r="AE2" s="51"/>
+      <c r="AF2" s="51"/>
+      <c r="AG2" s="51"/>
+      <c r="AH2" s="51"/>
     </row>
     <row r="3" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="40"/>
-      <c r="R3" s="40"/>
-      <c r="S3" s="40"/>
-      <c r="T3" s="40"/>
-      <c r="U3" s="40"/>
-      <c r="V3" s="40"/>
-      <c r="W3" s="40"/>
-      <c r="X3" s="40"/>
-      <c r="Y3" s="40"/>
-      <c r="Z3" s="40"/>
-      <c r="AA3" s="40"/>
-      <c r="AB3" s="40"/>
-      <c r="AC3" s="40"/>
-      <c r="AD3" s="40"/>
-      <c r="AE3" s="40"/>
-      <c r="AF3" s="40"/>
-      <c r="AG3" s="40"/>
-      <c r="AH3" s="40"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+      <c r="T3" s="51"/>
+      <c r="U3" s="51"/>
+      <c r="V3" s="51"/>
+      <c r="W3" s="51"/>
+      <c r="X3" s="51"/>
+      <c r="Y3" s="51"/>
+      <c r="Z3" s="51"/>
+      <c r="AA3" s="51"/>
+      <c r="AB3" s="51"/>
+      <c r="AC3" s="51"/>
+      <c r="AD3" s="51"/>
+      <c r="AE3" s="51"/>
+      <c r="AF3" s="51"/>
+      <c r="AG3" s="51"/>
+      <c r="AH3" s="51"/>
     </row>
     <row r="4" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
-      <c r="S4" s="40"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="40"/>
-      <c r="V4" s="40"/>
-      <c r="W4" s="40"/>
-      <c r="X4" s="40"/>
-      <c r="Y4" s="40"/>
-      <c r="Z4" s="40"/>
-      <c r="AA4" s="40"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="40"/>
-      <c r="AD4" s="40"/>
-      <c r="AE4" s="40"/>
-      <c r="AF4" s="40"/>
-      <c r="AG4" s="40"/>
-      <c r="AH4" s="40"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="51"/>
+      <c r="T4" s="51"/>
+      <c r="U4" s="51"/>
+      <c r="V4" s="51"/>
+      <c r="W4" s="51"/>
+      <c r="X4" s="51"/>
+      <c r="Y4" s="51"/>
+      <c r="Z4" s="51"/>
+      <c r="AA4" s="51"/>
+      <c r="AB4" s="51"/>
+      <c r="AC4" s="51"/>
+      <c r="AD4" s="51"/>
+      <c r="AE4" s="51"/>
+      <c r="AF4" s="51"/>
+      <c r="AG4" s="51"/>
+      <c r="AH4" s="51"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
-      <c r="V5" s="40"/>
-      <c r="W5" s="40"/>
-      <c r="X5" s="40"/>
-      <c r="Y5" s="40"/>
-      <c r="Z5" s="40"/>
-      <c r="AA5" s="40"/>
-      <c r="AB5" s="40"/>
-      <c r="AC5" s="40"/>
-      <c r="AD5" s="40"/>
-      <c r="AE5" s="40"/>
-      <c r="AF5" s="40"/>
-      <c r="AG5" s="40"/>
-      <c r="AH5" s="40"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="51"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="51"/>
+      <c r="U5" s="51"/>
+      <c r="V5" s="51"/>
+      <c r="W5" s="51"/>
+      <c r="X5" s="51"/>
+      <c r="Y5" s="51"/>
+      <c r="Z5" s="51"/>
+      <c r="AA5" s="51"/>
+      <c r="AB5" s="51"/>
+      <c r="AC5" s="51"/>
+      <c r="AD5" s="51"/>
+      <c r="AE5" s="51"/>
+      <c r="AF5" s="51"/>
+      <c r="AG5" s="51"/>
+      <c r="AH5" s="51"/>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="40"/>
-      <c r="S6" s="40"/>
-      <c r="T6" s="40"/>
-      <c r="U6" s="40"/>
-      <c r="V6" s="40"/>
-      <c r="W6" s="40"/>
-      <c r="X6" s="40"/>
-      <c r="Y6" s="40"/>
-      <c r="Z6" s="40"/>
-      <c r="AA6" s="40"/>
-      <c r="AB6" s="40"/>
-      <c r="AC6" s="40"/>
-      <c r="AD6" s="40"/>
-      <c r="AE6" s="40"/>
-      <c r="AF6" s="40"/>
-      <c r="AG6" s="40"/>
-      <c r="AH6" s="40"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="51"/>
+      <c r="R6" s="51"/>
+      <c r="S6" s="51"/>
+      <c r="T6" s="51"/>
+      <c r="U6" s="51"/>
+      <c r="V6" s="51"/>
+      <c r="W6" s="51"/>
+      <c r="X6" s="51"/>
+      <c r="Y6" s="51"/>
+      <c r="Z6" s="51"/>
+      <c r="AA6" s="51"/>
+      <c r="AB6" s="51"/>
+      <c r="AC6" s="51"/>
+      <c r="AD6" s="51"/>
+      <c r="AE6" s="51"/>
+      <c r="AF6" s="51"/>
+      <c r="AG6" s="51"/>
+      <c r="AH6" s="51"/>
     </row>
     <row r="7" spans="1:44" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="41" t="s">
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42"/>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="43"/>
-      <c r="R7" s="41" t="s">
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="42"/>
-      <c r="V7" s="42"/>
-      <c r="W7" s="42"/>
-      <c r="X7" s="42"/>
-      <c r="Y7" s="42"/>
-      <c r="Z7" s="42"/>
-      <c r="AA7" s="42"/>
-      <c r="AB7" s="42"/>
-      <c r="AC7" s="42"/>
-      <c r="AD7" s="42"/>
-      <c r="AE7" s="42"/>
-      <c r="AF7" s="42"/>
-      <c r="AG7" s="42"/>
-      <c r="AH7" s="43"/>
+      <c r="S7" s="53"/>
+      <c r="T7" s="53"/>
+      <c r="U7" s="53"/>
+      <c r="V7" s="53"/>
+      <c r="W7" s="53"/>
+      <c r="X7" s="53"/>
+      <c r="Y7" s="53"/>
+      <c r="Z7" s="53"/>
+      <c r="AA7" s="53"/>
+      <c r="AB7" s="53"/>
+      <c r="AC7" s="53"/>
+      <c r="AD7" s="53"/>
+      <c r="AE7" s="53"/>
+      <c r="AF7" s="53"/>
+      <c r="AG7" s="53"/>
+      <c r="AH7" s="54"/>
     </row>
     <row r="8" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="49"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
       <c r="E8" s="6">
         <v>16</v>
       </c>
@@ -1156,12 +1156,12 @@
       <c r="AL8" s="29"/>
     </row>
     <row r="9" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="7"/>
@@ -1194,12 +1194,12 @@
       <c r="AH9" s="7"/>
     </row>
     <row r="10" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="48"/>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -1232,12 +1232,12 @@
       <c r="AH10" s="14"/>
     </row>
     <row r="11" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
       <c r="E11" s="18"/>
       <c r="F11" s="25"/>
       <c r="G11" s="23"/>
@@ -1270,12 +1270,12 @@
       <c r="AH11" s="18"/>
     </row>
     <row r="12" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
       <c r="E12" s="18"/>
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
@@ -1308,51 +1308,51 @@
       <c r="AH12" s="18"/>
     </row>
     <row r="13" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="51"/>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="51"/>
-      <c r="S13" s="51"/>
-      <c r="T13" s="51"/>
-      <c r="U13" s="51"/>
-      <c r="V13" s="51"/>
-      <c r="W13" s="51"/>
-      <c r="X13" s="51"/>
-      <c r="Y13" s="51"/>
-      <c r="Z13" s="51"/>
-      <c r="AA13" s="51"/>
-      <c r="AB13" s="51"/>
-      <c r="AC13" s="51"/>
-      <c r="AD13" s="51"/>
-      <c r="AE13" s="51"/>
-      <c r="AF13" s="51"/>
-      <c r="AG13" s="51"/>
-      <c r="AH13" s="51"/>
-      <c r="AJ13" s="55"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="49"/>
+      <c r="U13" s="49"/>
+      <c r="V13" s="49"/>
+      <c r="W13" s="49"/>
+      <c r="X13" s="49"/>
+      <c r="Y13" s="49"/>
+      <c r="Z13" s="49"/>
+      <c r="AA13" s="49"/>
+      <c r="AB13" s="49"/>
+      <c r="AC13" s="49"/>
+      <c r="AD13" s="49"/>
+      <c r="AE13" s="49"/>
+      <c r="AF13" s="49"/>
+      <c r="AG13" s="49"/>
+      <c r="AH13" s="49"/>
+      <c r="AJ13" s="41"/>
     </row>
     <row r="14" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="50"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="44"/>
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
       <c r="G14" s="24"/>
@@ -1386,12 +1386,12 @@
       <c r="AR14" s="22"/>
     </row>
     <row r="15" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="50"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
@@ -1424,12 +1424,12 @@
       <c r="AH15" s="20"/>
     </row>
     <row r="16" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="50"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
@@ -1438,7 +1438,7 @@
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
       <c r="L16" s="20"/>
-      <c r="M16" s="53"/>
+      <c r="M16" s="39"/>
       <c r="N16" s="24"/>
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
@@ -1463,12 +1463,12 @@
       <c r="AP16" s="22"/>
     </row>
     <row r="17" spans="1:42" s="33" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="50"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="44"/>
       <c r="E17" s="34"/>
       <c r="F17" s="34"/>
       <c r="G17" s="34"/>
@@ -1503,12 +1503,12 @@
       <c r="AP17" s="22"/>
     </row>
     <row r="18" spans="1:42" s="33" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="50"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="44"/>
       <c r="E18" s="34"/>
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
@@ -1542,12 +1542,12 @@
       <c r="AP18" s="22"/>
     </row>
     <row r="19" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
@@ -1580,12 +1580,12 @@
       <c r="AH19" s="18"/>
     </row>
     <row r="20" spans="1:42" s="27" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="50"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="44"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
@@ -1598,7 +1598,7 @@
       <c r="N20" s="23"/>
       <c r="O20" s="23"/>
       <c r="P20" s="23"/>
-      <c r="Q20" s="54"/>
+      <c r="Q20" s="40"/>
       <c r="R20" s="24"/>
       <c r="S20" s="18"/>
       <c r="T20" s="18"/>
@@ -1618,12 +1618,12 @@
       <c r="AH20" s="18"/>
     </row>
     <row r="21" spans="1:42" s="27" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="50"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="44"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
@@ -1636,7 +1636,7 @@
       <c r="N21" s="24"/>
       <c r="O21" s="24"/>
       <c r="P21" s="24"/>
-      <c r="Q21" s="54"/>
+      <c r="Q21" s="40"/>
       <c r="R21" s="24"/>
       <c r="S21" s="18"/>
       <c r="T21" s="18"/>
@@ -1656,12 +1656,12 @@
       <c r="AH21" s="18"/>
     </row>
     <row r="22" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="46"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="16"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
@@ -1695,12 +1695,12 @@
       <c r="AN22" s="22"/>
     </row>
     <row r="23" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="50"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="44"/>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
@@ -1734,12 +1734,12 @@
       <c r="AL23" s="22"/>
     </row>
     <row r="24" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="47" t="s">
+      <c r="A24" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="50"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="44"/>
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -1772,12 +1772,12 @@
       <c r="AH24" s="19"/>
     </row>
     <row r="25" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="47" t="s">
+      <c r="A25" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="50"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="44"/>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
@@ -1810,12 +1810,12 @@
       <c r="AH25" s="19"/>
     </row>
     <row r="26" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="46"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="48"/>
       <c r="E26" s="9"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
@@ -1848,12 +1848,12 @@
       <c r="AH26" s="11"/>
     </row>
     <row r="27" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="50"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="44"/>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
@@ -1886,12 +1886,12 @@
       <c r="AH27" s="19"/>
     </row>
     <row r="28" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="50"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
@@ -1924,12 +1924,12 @@
       <c r="AH28" s="4"/>
     </row>
     <row r="29" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="50"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="44"/>
       <c r="E29" s="5"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -1962,12 +1962,12 @@
       <c r="AH29" s="3"/>
     </row>
     <row r="30" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
       <c r="E30" s="4"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -2000,34 +2000,19 @@
       <c r="AH30" s="3"/>
     </row>
     <row r="34" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
     </row>
     <row r="35" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E35" s="52"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E13:AH13"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A14:D14"/>
     <mergeCell ref="E1:AH6"/>
     <mergeCell ref="E7:Q7"/>
     <mergeCell ref="R7:AH7"/>
@@ -2042,6 +2027,21 @@
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E13:AH13"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>